<commit_message>
Updating all the component code and results from analyses
</commit_message>
<xml_diff>
--- a/3_Results/32_ResultsVMMC/vmmc_three_way_tables.xlsx
+++ b/3_Results/32_ResultsVMMC/vmmc_three_way_tables.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Y1 by X1 Individual" sheetId="1" r:id="rId1"/>
     <sheet name="Y1 by Z1 Spillover" sheetId="2" r:id="rId2"/>
-    <sheet name="Y1 by X1 Overall" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -852,324 +851,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Treatment</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Outcome</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>70</v>
-      </c>
-      <c r="F2">
-        <v>90</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="C3">
-        <v>579</v>
-      </c>
-      <c r="D3">
-        <v>864</v>
-      </c>
-      <c r="E3">
-        <v>2543</v>
-      </c>
-      <c r="F3">
-        <v>3986</v>
-      </c>
-      <c r="G3">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C4">
-        <v>584</v>
-      </c>
-      <c r="D4">
-        <v>879</v>
-      </c>
-      <c r="E4">
-        <v>3948</v>
-      </c>
-      <c r="F4">
-        <v>5411</v>
-      </c>
-      <c r="G4">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>81</v>
-      </c>
-      <c r="D5">
-        <v>112</v>
-      </c>
-      <c r="E5">
-        <v>214</v>
-      </c>
-      <c r="F5">
-        <v>407</v>
-      </c>
-      <c r="G5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Began study HIV-infected</t>
-        </is>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1335</v>
-      </c>
-      <c r="F6">
-        <v>1335</v>
-      </c>
-      <c r="G6">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Treatment</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>49</v>
-      </c>
-      <c r="F7">
-        <v>57</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Treatment</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="C8">
-        <v>750</v>
-      </c>
-      <c r="D8">
-        <v>689</v>
-      </c>
-      <c r="E8">
-        <v>2537</v>
-      </c>
-      <c r="F8">
-        <v>3976</v>
-      </c>
-      <c r="G8">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Treatment</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C9">
-        <v>753</v>
-      </c>
-      <c r="D9">
-        <v>695</v>
-      </c>
-      <c r="E9">
-        <v>3933</v>
-      </c>
-      <c r="F9">
-        <v>5381</v>
-      </c>
-      <c r="G9">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Treatment</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Missing</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10">
-        <v>107</v>
-      </c>
-      <c r="E10">
-        <v>245</v>
-      </c>
-      <c r="F10">
-        <v>452</v>
-      </c>
-      <c r="G10">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Treatment</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Began study HIV-infected</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1347</v>
-      </c>
-      <c r="F11">
-        <v>1348</v>
-      </c>
-      <c r="G11">
-        <v>506</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>